<commit_message>
Updates to JLCPCB format
</commit_message>
<xml_diff>
--- a/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
+++ b/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\System\pcb\rev2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\Maker\aqp-rev2\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C6DEB5-51A8-4D06-A050-992823198030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3253D-74CA-4C96-8F1F-9C4343829830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>

</xml_diff>

<commit_message>
Altered audio jacks for different JLCPCB part num
</commit_message>
<xml_diff>
--- a/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
+++ b/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\Maker\aqp-rev2\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC3253D-74CA-4C96-8F1F-9C4343829830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0C7377-9172-442D-A03A-D1DCAB517651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,18 +510,12 @@
     <t>C138387</t>
   </si>
   <si>
-    <t>PJ-320B-SMT</t>
-  </si>
-  <si>
     <t>C2913203</t>
   </si>
   <si>
     <t>C7431259</t>
   </si>
   <si>
-    <t>C2939180</t>
-  </si>
-  <si>
     <t>J11,J12</t>
   </si>
   <si>
@@ -538,6 +532,12 @@
   </si>
   <si>
     <t>J3,J5,J6,J8</t>
+  </si>
+  <si>
+    <t>C2689690</t>
+  </si>
+  <si>
+    <t>PJ-3200</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1466,29 +1466,29 @@
         <v>103</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15">
       <c r="A33" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B33" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="57">
       <c r="A34" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>102</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="41" spans="1:4" ht="15">
       <c r="A41" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>108</v>
@@ -1620,7 +1620,7 @@
         <v>105</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15">

</xml_diff>

<commit_message>
Updates to TheValley & rev2 BOM
</commit_message>
<xml_diff>
--- a/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
+++ b/Maker/aqp-rev2/pcb/aqplus_rev2_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sph\Box\Retro\Aquarius\AquariusPlus\aquarius-plus\Maker\aqp-rev2\pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65D93E1-8A3C-4865-83A1-39159480FAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276746D6-0457-4B0F-B420-B096F1728BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7095" yWindow="2700" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="160">
   <si>
     <t>Comment</t>
   </si>
@@ -364,9 +364,6 @@
   </si>
   <si>
     <t>DSUB-9_Male_Horizontal_P2.77x2.84mm_EdgePinOffset9.90mm_Housed_MountingHolesOffset11.32mm</t>
-  </si>
-  <si>
-    <t>ESP32-S2-SOLO-N4R2</t>
   </si>
   <si>
     <t>C_0603_1608Metric</t>
@@ -1001,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="20.100000000000001" customHeight="1"/>
@@ -1039,7 +1036,7 @@
         <v>101</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" s="6"/>
     </row>
@@ -1054,7 +1051,7 @@
         <v>90</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E3" s="6"/>
     </row>
@@ -1069,7 +1066,7 @@
         <v>87</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E4" s="6"/>
     </row>
@@ -1084,7 +1081,7 @@
         <v>94</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E5" s="6"/>
     </row>
@@ -1096,10 +1093,10 @@
         <v>55</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E6" s="6"/>
     </row>
@@ -1114,7 +1111,7 @@
         <v>95</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E7" s="6"/>
     </row>
@@ -1129,7 +1126,7 @@
         <v>91</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E8" s="6"/>
     </row>
@@ -1144,7 +1141,7 @@
         <v>86</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15">
@@ -1158,7 +1155,7 @@
         <v>87</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15">
@@ -1172,7 +1169,7 @@
         <v>88</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="85.5">
@@ -1183,10 +1180,10 @@
         <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="42.75">
@@ -1200,7 +1197,7 @@
         <v>87</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15">
@@ -1214,7 +1211,7 @@
         <v>99</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="128.25">
@@ -1228,7 +1225,7 @@
         <v>87</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
@@ -1242,7 +1239,7 @@
         <v>87</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15">
@@ -1256,7 +1253,7 @@
         <v>87</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15">
@@ -1270,7 +1267,7 @@
         <v>87</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15">
@@ -1284,7 +1281,7 @@
         <v>87</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15">
@@ -1298,7 +1295,7 @@
         <v>87</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15">
@@ -1312,7 +1309,7 @@
         <v>87</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15">
@@ -1326,7 +1323,7 @@
         <v>87</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="28.5">
@@ -1340,7 +1337,7 @@
         <v>87</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15">
@@ -1354,7 +1351,7 @@
         <v>87</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="42.75">
@@ -1368,7 +1365,7 @@
         <v>87</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15">
@@ -1382,7 +1379,7 @@
         <v>87</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15">
@@ -1396,7 +1393,7 @@
         <v>93</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15">
@@ -1410,7 +1407,7 @@
         <v>98</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15">
@@ -1421,10 +1418,10 @@
         <v>57</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15">
@@ -1438,7 +1435,7 @@
         <v>96</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.5">
@@ -1452,7 +1449,7 @@
         <v>100</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15">
@@ -1462,39 +1459,39 @@
       <c r="B32" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C32" s="9" t="s">
-        <v>103</v>
+      <c r="C32" s="4" t="s">
+        <v>44</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15">
       <c r="A33" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B33" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="C33" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D33" s="7" t="s">
         <v>156</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="57">
       <c r="A34" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B34" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>102</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.5">
@@ -1508,7 +1505,7 @@
         <v>97</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15">
@@ -1519,10 +1516,10 @@
         <v>51</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15">
@@ -1536,7 +1533,7 @@
         <v>89</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15">
@@ -1550,7 +1547,7 @@
         <v>87</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15">
@@ -1564,7 +1561,7 @@
         <v>91</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15">
@@ -1575,24 +1572,24 @@
         <v>52</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15">
       <c r="A41" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B41" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B41" s="9" t="s">
-        <v>154</v>
-      </c>
       <c r="C41" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15">
@@ -1606,7 +1603,7 @@
         <v>34</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15">
@@ -1617,10 +1614,10 @@
         <v>48</v>
       </c>
       <c r="C43" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15">
@@ -1634,7 +1631,7 @@
         <v>92</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15">
@@ -1648,7 +1645,7 @@
         <v>88</v>
       </c>
       <c r="D45" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>